<commit_message>
fixing perhitungan total working hours
</commit_message>
<xml_diff>
--- a/output/report_9_Juli_-_26_September_2024.xlsx
+++ b/output/report_9_Juli_-_26_September_2024.xlsx
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="D3" s="22" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
     </row>
     <row r="4">
@@ -9957,8 +9957,10 @@
           <t>FITTER</t>
         </is>
       </c>
-      <c r="D83" t="n">
-        <v/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>H162</t>
+        </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -9967,12 +9969,12 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:48</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -9990,28 +9992,28 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P83" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q83" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="R83" t="inlineStr">
         <is>
@@ -23761,19 +23763,19 @@
         <v>1</v>
       </c>
       <c r="O82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P82" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q82" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R82" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S82" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T82" t="n">
         <v>0</v>
@@ -23785,7 +23787,7 @@
         <v>0</v>
       </c>
       <c r="W82" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X82" t="inlineStr">
         <is>
@@ -23844,31 +23846,31 @@
         </is>
       </c>
       <c r="K83" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="L83" t="n">
-        <v>0</v>
+        <v>178500</v>
       </c>
       <c r="M83" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="N83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P83" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q83" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R83" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S83" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T83" t="n">
         <v>0</v>
@@ -23880,15 +23882,17 @@
         <v>0</v>
       </c>
       <c r="W83" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X83" t="inlineStr">
         <is>
           <t>57600_HENGKI_BOY_HUTASOIT</t>
         </is>
       </c>
-      <c r="Y83" t="n">
-        <v/>
+      <c r="Y83" t="inlineStr">
+        <is>
+          <t>H162</t>
+        </is>
       </c>
     </row>
     <row r="84">
@@ -23949,19 +23953,19 @@
         <v>0</v>
       </c>
       <c r="O84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P84" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q84" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R84" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S84" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T84" t="n">
         <v>0</v>
@@ -23973,7 +23977,7 @@
         <v>0</v>
       </c>
       <c r="W84" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X84" t="inlineStr">
         <is>
@@ -24042,19 +24046,19 @@
         <v>0</v>
       </c>
       <c r="O85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P85" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q85" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R85" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S85" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T85" t="n">
         <v>0</v>
@@ -24066,7 +24070,7 @@
         <v>0</v>
       </c>
       <c r="W85" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X85" t="inlineStr">
         <is>
@@ -24135,19 +24139,19 @@
         <v>0</v>
       </c>
       <c r="O86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P86" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q86" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R86" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S86" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T86" t="n">
         <v>0</v>
@@ -24159,7 +24163,7 @@
         <v>0</v>
       </c>
       <c r="W86" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X86" t="inlineStr">
         <is>
@@ -24228,19 +24232,19 @@
         <v>0</v>
       </c>
       <c r="O87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P87" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q87" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R87" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S87" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T87" t="n">
         <v>0</v>
@@ -24252,7 +24256,7 @@
         <v>0</v>
       </c>
       <c r="W87" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X87" t="inlineStr">
         <is>
@@ -24321,19 +24325,19 @@
         <v>0</v>
       </c>
       <c r="O88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P88" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q88" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R88" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S88" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T88" t="n">
         <v>0</v>
@@ -24345,7 +24349,7 @@
         <v>0</v>
       </c>
       <c r="W88" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X88" t="inlineStr">
         <is>
@@ -24414,19 +24418,19 @@
         <v>0</v>
       </c>
       <c r="O89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P89" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q89" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R89" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S89" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T89" t="n">
         <v>0</v>
@@ -24438,7 +24442,7 @@
         <v>0</v>
       </c>
       <c r="W89" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X89" t="inlineStr">
         <is>
@@ -24507,19 +24511,19 @@
         <v>0</v>
       </c>
       <c r="O90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P90" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q90" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R90" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S90" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T90" t="n">
         <v>0</v>
@@ -24531,7 +24535,7 @@
         <v>0</v>
       </c>
       <c r="W90" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X90" t="inlineStr">
         <is>
@@ -24600,19 +24604,19 @@
         <v>0</v>
       </c>
       <c r="O91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P91" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q91" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R91" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S91" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T91" t="n">
         <v>0</v>
@@ -24624,7 +24628,7 @@
         <v>0</v>
       </c>
       <c r="W91" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X91" t="inlineStr">
         <is>
@@ -24693,19 +24697,19 @@
         <v>0</v>
       </c>
       <c r="O92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P92" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q92" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R92" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S92" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T92" t="n">
         <v>0</v>
@@ -24717,7 +24721,7 @@
         <v>0</v>
       </c>
       <c r="W92" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X92" t="inlineStr">
         <is>
@@ -24786,19 +24790,19 @@
         <v>0</v>
       </c>
       <c r="O93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P93" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q93" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R93" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S93" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T93" t="n">
         <v>0</v>
@@ -24810,7 +24814,7 @@
         <v>0</v>
       </c>
       <c r="W93" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X93" t="inlineStr">
         <is>
@@ -24879,19 +24883,19 @@
         <v>0</v>
       </c>
       <c r="O94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P94" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q94" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R94" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S94" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T94" t="n">
         <v>0</v>
@@ -24903,7 +24907,7 @@
         <v>0</v>
       </c>
       <c r="W94" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X94" t="inlineStr">
         <is>
@@ -24972,19 +24976,19 @@
         <v>0</v>
       </c>
       <c r="O95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P95" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q95" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R95" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S95" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T95" t="n">
         <v>0</v>
@@ -24996,7 +25000,7 @@
         <v>0</v>
       </c>
       <c r="W95" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X95" t="inlineStr">
         <is>
@@ -25065,19 +25069,19 @@
         <v>0</v>
       </c>
       <c r="O96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P96" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q96" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R96" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S96" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T96" t="n">
         <v>0</v>
@@ -25089,7 +25093,7 @@
         <v>0</v>
       </c>
       <c r="W96" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X96" t="inlineStr">
         <is>
@@ -25158,19 +25162,19 @@
         <v>0</v>
       </c>
       <c r="O97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P97" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q97" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R97" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S97" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T97" t="n">
         <v>0</v>
@@ -25182,7 +25186,7 @@
         <v>0</v>
       </c>
       <c r="W97" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X97" t="inlineStr">
         <is>
@@ -25251,19 +25255,19 @@
         <v>0</v>
       </c>
       <c r="O98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P98" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q98" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R98" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S98" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T98" t="n">
         <v>0</v>
@@ -25275,7 +25279,7 @@
         <v>0</v>
       </c>
       <c r="W98" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X98" t="inlineStr">
         <is>
@@ -25344,19 +25348,19 @@
         <v>0</v>
       </c>
       <c r="O99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P99" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q99" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R99" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S99" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T99" t="n">
         <v>0</v>
@@ -25368,7 +25372,7 @@
         <v>0</v>
       </c>
       <c r="W99" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X99" t="inlineStr">
         <is>
@@ -25437,19 +25441,19 @@
         <v>0</v>
       </c>
       <c r="O100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P100" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q100" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R100" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S100" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T100" t="n">
         <v>0</v>
@@ -25461,7 +25465,7 @@
         <v>0</v>
       </c>
       <c r="W100" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X100" t="inlineStr">
         <is>
@@ -25530,19 +25534,19 @@
         <v>0</v>
       </c>
       <c r="O101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P101" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q101" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R101" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S101" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T101" t="n">
         <v>0</v>
@@ -25554,7 +25558,7 @@
         <v>0</v>
       </c>
       <c r="W101" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X101" t="inlineStr">
         <is>
@@ -25623,19 +25627,19 @@
         <v>0</v>
       </c>
       <c r="O102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P102" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q102" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R102" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S102" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T102" t="n">
         <v>0</v>
@@ -25647,7 +25651,7 @@
         <v>0</v>
       </c>
       <c r="W102" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X102" t="inlineStr">
         <is>
@@ -25716,19 +25720,19 @@
         <v>0</v>
       </c>
       <c r="O103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P103" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q103" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R103" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S103" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T103" t="n">
         <v>0</v>
@@ -25740,7 +25744,7 @@
         <v>0</v>
       </c>
       <c r="W103" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X103" t="inlineStr">
         <is>
@@ -25809,19 +25813,19 @@
         <v>0</v>
       </c>
       <c r="O104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P104" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q104" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R104" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S104" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T104" t="n">
         <v>0</v>
@@ -25833,7 +25837,7 @@
         <v>0</v>
       </c>
       <c r="W104" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X104" t="inlineStr">
         <is>
@@ -25902,19 +25906,19 @@
         <v>0</v>
       </c>
       <c r="O105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P105" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q105" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R105" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S105" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T105" t="n">
         <v>0</v>
@@ -25926,7 +25930,7 @@
         <v>0</v>
       </c>
       <c r="W105" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X105" t="inlineStr">
         <is>
@@ -25995,19 +25999,19 @@
         <v>0</v>
       </c>
       <c r="O106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P106" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q106" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R106" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S106" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T106" t="n">
         <v>0</v>
@@ -26019,7 +26023,7 @@
         <v>0</v>
       </c>
       <c r="W106" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X106" t="inlineStr">
         <is>
@@ -26088,19 +26092,19 @@
         <v>0</v>
       </c>
       <c r="O107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P107" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q107" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R107" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S107" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T107" t="n">
         <v>0</v>
@@ -26112,7 +26116,7 @@
         <v>0</v>
       </c>
       <c r="W107" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X107" t="inlineStr">
         <is>
@@ -26181,19 +26185,19 @@
         <v>0</v>
       </c>
       <c r="O108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P108" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q108" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R108" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S108" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T108" t="n">
         <v>0</v>
@@ -26205,7 +26209,7 @@
         <v>0</v>
       </c>
       <c r="W108" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X108" t="inlineStr">
         <is>
@@ -26274,19 +26278,19 @@
         <v>0</v>
       </c>
       <c r="O109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P109" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q109" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R109" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S109" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T109" t="n">
         <v>0</v>
@@ -26298,7 +26302,7 @@
         <v>0</v>
       </c>
       <c r="W109" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X109" t="inlineStr">
         <is>
@@ -26367,19 +26371,19 @@
         <v>0</v>
       </c>
       <c r="O110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P110" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q110" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R110" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S110" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T110" t="n">
         <v>0</v>
@@ -26391,7 +26395,7 @@
         <v>0</v>
       </c>
       <c r="W110" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X110" t="inlineStr">
         <is>
@@ -26460,19 +26464,19 @@
         <v>0</v>
       </c>
       <c r="O111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P111" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q111" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R111" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S111" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T111" t="n">
         <v>0</v>
@@ -26484,7 +26488,7 @@
         <v>0</v>
       </c>
       <c r="W111" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X111" t="inlineStr">
         <is>
@@ -26553,19 +26557,19 @@
         <v>0</v>
       </c>
       <c r="O112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P112" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q112" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R112" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S112" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T112" t="n">
         <v>0</v>
@@ -26577,7 +26581,7 @@
         <v>0</v>
       </c>
       <c r="W112" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X112" t="inlineStr">
         <is>
@@ -26646,19 +26650,19 @@
         <v>0</v>
       </c>
       <c r="O113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P113" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q113" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R113" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S113" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T113" t="n">
         <v>0</v>
@@ -26670,7 +26674,7 @@
         <v>0</v>
       </c>
       <c r="W113" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X113" t="inlineStr">
         <is>
@@ -26739,19 +26743,19 @@
         <v>0</v>
       </c>
       <c r="O114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P114" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q114" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R114" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S114" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T114" t="n">
         <v>0</v>
@@ -26763,7 +26767,7 @@
         <v>0</v>
       </c>
       <c r="W114" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X114" t="inlineStr">
         <is>
@@ -26832,19 +26836,19 @@
         <v>0</v>
       </c>
       <c r="O115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P115" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q115" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R115" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S115" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T115" t="n">
         <v>0</v>
@@ -26856,7 +26860,7 @@
         <v>0</v>
       </c>
       <c r="W115" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X115" t="inlineStr">
         <is>
@@ -26925,19 +26929,19 @@
         <v>0</v>
       </c>
       <c r="O116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P116" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q116" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R116" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S116" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T116" t="n">
         <v>0</v>
@@ -26949,7 +26953,7 @@
         <v>0</v>
       </c>
       <c r="W116" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X116" t="inlineStr">
         <is>
@@ -27018,19 +27022,19 @@
         <v>0</v>
       </c>
       <c r="O117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P117" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q117" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R117" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S117" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T117" t="n">
         <v>0</v>
@@ -27042,7 +27046,7 @@
         <v>0</v>
       </c>
       <c r="W117" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X117" t="inlineStr">
         <is>
@@ -27111,19 +27115,19 @@
         <v>0</v>
       </c>
       <c r="O118" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P118" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q118" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R118" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S118" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T118" t="n">
         <v>0</v>
@@ -27135,7 +27139,7 @@
         <v>0</v>
       </c>
       <c r="W118" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X118" t="inlineStr">
         <is>
@@ -27204,19 +27208,19 @@
         <v>0</v>
       </c>
       <c r="O119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P119" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q119" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R119" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S119" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T119" t="n">
         <v>0</v>
@@ -27228,7 +27232,7 @@
         <v>0</v>
       </c>
       <c r="W119" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X119" t="inlineStr">
         <is>
@@ -27297,19 +27301,19 @@
         <v>0</v>
       </c>
       <c r="O120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P120" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q120" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R120" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S120" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T120" t="n">
         <v>0</v>
@@ -27321,7 +27325,7 @@
         <v>0</v>
       </c>
       <c r="W120" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X120" t="inlineStr">
         <is>
@@ -27390,19 +27394,19 @@
         <v>0</v>
       </c>
       <c r="O121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P121" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q121" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R121" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S121" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T121" t="n">
         <v>0</v>
@@ -27414,7 +27418,7 @@
         <v>0</v>
       </c>
       <c r="W121" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X121" t="inlineStr">
         <is>
@@ -27483,19 +27487,19 @@
         <v>0</v>
       </c>
       <c r="O122" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P122" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q122" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R122" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S122" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T122" t="n">
         <v>0</v>
@@ -27507,7 +27511,7 @@
         <v>0</v>
       </c>
       <c r="W122" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X122" t="inlineStr">
         <is>
@@ -27576,19 +27580,19 @@
         <v>0</v>
       </c>
       <c r="O123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P123" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q123" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R123" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S123" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T123" t="n">
         <v>0</v>
@@ -27600,7 +27604,7 @@
         <v>0</v>
       </c>
       <c r="W123" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X123" t="inlineStr">
         <is>
@@ -27669,19 +27673,19 @@
         <v>0</v>
       </c>
       <c r="O124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P124" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q124" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R124" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S124" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T124" t="n">
         <v>0</v>
@@ -27693,7 +27697,7 @@
         <v>0</v>
       </c>
       <c r="W124" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X124" t="inlineStr">
         <is>
@@ -27762,19 +27766,19 @@
         <v>0</v>
       </c>
       <c r="O125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P125" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q125" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R125" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S125" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T125" t="n">
         <v>0</v>
@@ -27786,7 +27790,7 @@
         <v>0</v>
       </c>
       <c r="W125" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X125" t="inlineStr">
         <is>
@@ -27855,19 +27859,19 @@
         <v>0</v>
       </c>
       <c r="O126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P126" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q126" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R126" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S126" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T126" t="n">
         <v>0</v>
@@ -27879,7 +27883,7 @@
         <v>0</v>
       </c>
       <c r="W126" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X126" t="inlineStr">
         <is>
@@ -27948,19 +27952,19 @@
         <v>0</v>
       </c>
       <c r="O127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P127" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q127" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R127" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S127" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T127" t="n">
         <v>0</v>
@@ -27972,7 +27976,7 @@
         <v>0</v>
       </c>
       <c r="W127" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X127" t="inlineStr">
         <is>
@@ -28041,19 +28045,19 @@
         <v>0</v>
       </c>
       <c r="O128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P128" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q128" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R128" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S128" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T128" t="n">
         <v>0</v>
@@ -28065,7 +28069,7 @@
         <v>0</v>
       </c>
       <c r="W128" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X128" t="inlineStr">
         <is>
@@ -28134,19 +28138,19 @@
         <v>0</v>
       </c>
       <c r="O129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P129" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q129" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R129" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S129" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T129" t="n">
         <v>0</v>
@@ -28158,7 +28162,7 @@
         <v>0</v>
       </c>
       <c r="W129" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X129" t="inlineStr">
         <is>
@@ -28227,19 +28231,19 @@
         <v>0</v>
       </c>
       <c r="O130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P130" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q130" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R130" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S130" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T130" t="n">
         <v>0</v>
@@ -28251,7 +28255,7 @@
         <v>0</v>
       </c>
       <c r="W130" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X130" t="inlineStr">
         <is>
@@ -28320,19 +28324,19 @@
         <v>0</v>
       </c>
       <c r="O131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P131" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q131" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R131" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S131" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T131" t="n">
         <v>0</v>
@@ -28344,7 +28348,7 @@
         <v>0</v>
       </c>
       <c r="W131" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X131" t="inlineStr">
         <is>
@@ -28413,19 +28417,19 @@
         <v>0</v>
       </c>
       <c r="O132" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P132" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q132" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R132" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S132" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T132" t="n">
         <v>0</v>
@@ -28437,7 +28441,7 @@
         <v>0</v>
       </c>
       <c r="W132" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X132" t="inlineStr">
         <is>
@@ -28506,19 +28510,19 @@
         <v>0</v>
       </c>
       <c r="O133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P133" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q133" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R133" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S133" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T133" t="n">
         <v>0</v>
@@ -28530,7 +28534,7 @@
         <v>0</v>
       </c>
       <c r="W133" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X133" t="inlineStr">
         <is>
@@ -28599,19 +28603,19 @@
         <v>0</v>
       </c>
       <c r="O134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P134" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q134" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R134" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S134" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T134" t="n">
         <v>0</v>
@@ -28623,7 +28627,7 @@
         <v>0</v>
       </c>
       <c r="W134" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X134" t="inlineStr">
         <is>
@@ -28692,19 +28696,19 @@
         <v>0</v>
       </c>
       <c r="O135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P135" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q135" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R135" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S135" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T135" t="n">
         <v>0</v>
@@ -28716,7 +28720,7 @@
         <v>0</v>
       </c>
       <c r="W135" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X135" t="inlineStr">
         <is>
@@ -28785,19 +28789,19 @@
         <v>0</v>
       </c>
       <c r="O136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P136" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q136" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R136" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S136" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T136" t="n">
         <v>0</v>
@@ -28809,7 +28813,7 @@
         <v>0</v>
       </c>
       <c r="W136" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X136" t="inlineStr">
         <is>
@@ -28878,19 +28882,19 @@
         <v>0</v>
       </c>
       <c r="O137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P137" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q137" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R137" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S137" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T137" t="n">
         <v>0</v>
@@ -28902,7 +28906,7 @@
         <v>0</v>
       </c>
       <c r="W137" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X137" t="inlineStr">
         <is>
@@ -28971,19 +28975,19 @@
         <v>0</v>
       </c>
       <c r="O138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P138" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q138" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R138" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S138" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T138" t="n">
         <v>0</v>
@@ -28995,7 +28999,7 @@
         <v>0</v>
       </c>
       <c r="W138" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X138" t="inlineStr">
         <is>
@@ -29064,19 +29068,19 @@
         <v>0</v>
       </c>
       <c r="O139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P139" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q139" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R139" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S139" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T139" t="n">
         <v>0</v>
@@ -29088,7 +29092,7 @@
         <v>0</v>
       </c>
       <c r="W139" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X139" t="inlineStr">
         <is>
@@ -29157,19 +29161,19 @@
         <v>0</v>
       </c>
       <c r="O140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P140" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q140" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R140" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S140" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T140" t="n">
         <v>0</v>
@@ -29181,7 +29185,7 @@
         <v>0</v>
       </c>
       <c r="W140" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X140" t="inlineStr">
         <is>
@@ -29250,19 +29254,19 @@
         <v>0</v>
       </c>
       <c r="O141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P141" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q141" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R141" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S141" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T141" t="n">
         <v>0</v>
@@ -29274,7 +29278,7 @@
         <v>0</v>
       </c>
       <c r="W141" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X141" t="inlineStr">
         <is>
@@ -29343,19 +29347,19 @@
         <v>0</v>
       </c>
       <c r="O142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P142" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q142" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R142" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S142" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T142" t="n">
         <v>0</v>
@@ -29367,7 +29371,7 @@
         <v>0</v>
       </c>
       <c r="W142" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X142" t="inlineStr">
         <is>
@@ -29436,19 +29440,19 @@
         <v>0</v>
       </c>
       <c r="O143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P143" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q143" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R143" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S143" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T143" t="n">
         <v>0</v>
@@ -29460,7 +29464,7 @@
         <v>0</v>
       </c>
       <c r="W143" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X143" t="inlineStr">
         <is>
@@ -29529,19 +29533,19 @@
         <v>0</v>
       </c>
       <c r="O144" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P144" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q144" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R144" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S144" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T144" t="n">
         <v>0</v>
@@ -29553,7 +29557,7 @@
         <v>0</v>
       </c>
       <c r="W144" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X144" t="inlineStr">
         <is>
@@ -29622,19 +29626,19 @@
         <v>0</v>
       </c>
       <c r="O145" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P145" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q145" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R145" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S145" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T145" t="n">
         <v>0</v>
@@ -29646,7 +29650,7 @@
         <v>0</v>
       </c>
       <c r="W145" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X145" t="inlineStr">
         <is>
@@ -29715,19 +29719,19 @@
         <v>0</v>
       </c>
       <c r="O146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P146" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q146" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R146" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S146" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T146" t="n">
         <v>0</v>
@@ -29739,7 +29743,7 @@
         <v>0</v>
       </c>
       <c r="W146" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X146" t="inlineStr">
         <is>
@@ -29808,19 +29812,19 @@
         <v>0</v>
       </c>
       <c r="O147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P147" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q147" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R147" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S147" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T147" t="n">
         <v>0</v>
@@ -29832,7 +29836,7 @@
         <v>0</v>
       </c>
       <c r="W147" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X147" t="inlineStr">
         <is>
@@ -29901,19 +29905,19 @@
         <v>0</v>
       </c>
       <c r="O148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P148" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q148" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R148" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S148" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T148" t="n">
         <v>0</v>
@@ -29925,7 +29929,7 @@
         <v>0</v>
       </c>
       <c r="W148" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X148" t="inlineStr">
         <is>
@@ -29994,19 +29998,19 @@
         <v>0</v>
       </c>
       <c r="O149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P149" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q149" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R149" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S149" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T149" t="n">
         <v>0</v>
@@ -30018,7 +30022,7 @@
         <v>0</v>
       </c>
       <c r="W149" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X149" t="inlineStr">
         <is>
@@ -30087,19 +30091,19 @@
         <v>0</v>
       </c>
       <c r="O150" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P150" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q150" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R150" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S150" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T150" t="n">
         <v>0</v>
@@ -30111,7 +30115,7 @@
         <v>0</v>
       </c>
       <c r="W150" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X150" t="inlineStr">
         <is>
@@ -30180,19 +30184,19 @@
         <v>0</v>
       </c>
       <c r="O151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P151" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q151" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R151" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S151" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T151" t="n">
         <v>0</v>
@@ -30204,7 +30208,7 @@
         <v>0</v>
       </c>
       <c r="W151" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X151" t="inlineStr">
         <is>
@@ -30273,19 +30277,19 @@
         <v>0</v>
       </c>
       <c r="O152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P152" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q152" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R152" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S152" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T152" t="n">
         <v>0</v>
@@ -30297,7 +30301,7 @@
         <v>0</v>
       </c>
       <c r="W152" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X152" t="inlineStr">
         <is>
@@ -30366,19 +30370,19 @@
         <v>0</v>
       </c>
       <c r="O153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P153" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q153" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R153" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S153" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T153" t="n">
         <v>0</v>
@@ -30390,7 +30394,7 @@
         <v>0</v>
       </c>
       <c r="W153" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X153" t="inlineStr">
         <is>
@@ -30459,19 +30463,19 @@
         <v>0</v>
       </c>
       <c r="O154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P154" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q154" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R154" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S154" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T154" t="n">
         <v>0</v>
@@ -30483,7 +30487,7 @@
         <v>0</v>
       </c>
       <c r="W154" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X154" t="inlineStr">
         <is>
@@ -30552,19 +30556,19 @@
         <v>0</v>
       </c>
       <c r="O155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P155" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q155" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R155" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S155" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T155" t="n">
         <v>0</v>
@@ -30576,7 +30580,7 @@
         <v>0</v>
       </c>
       <c r="W155" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X155" t="inlineStr">
         <is>
@@ -30645,19 +30649,19 @@
         <v>0</v>
       </c>
       <c r="O156" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P156" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q156" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R156" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S156" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T156" t="n">
         <v>0</v>
@@ -30669,7 +30673,7 @@
         <v>0</v>
       </c>
       <c r="W156" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X156" t="inlineStr">
         <is>
@@ -30738,19 +30742,19 @@
         <v>0</v>
       </c>
       <c r="O157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P157" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q157" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R157" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S157" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T157" t="n">
         <v>0</v>
@@ -30762,7 +30766,7 @@
         <v>0</v>
       </c>
       <c r="W157" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X157" t="inlineStr">
         <is>
@@ -30831,19 +30835,19 @@
         <v>0</v>
       </c>
       <c r="O158" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P158" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q158" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R158" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S158" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T158" t="n">
         <v>0</v>
@@ -30855,7 +30859,7 @@
         <v>0</v>
       </c>
       <c r="W158" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X158" t="inlineStr">
         <is>
@@ -30924,19 +30928,19 @@
         <v>0</v>
       </c>
       <c r="O159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P159" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q159" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R159" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S159" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T159" t="n">
         <v>0</v>
@@ -30948,7 +30952,7 @@
         <v>0</v>
       </c>
       <c r="W159" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X159" t="inlineStr">
         <is>
@@ -31017,19 +31021,19 @@
         <v>0</v>
       </c>
       <c r="O160" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P160" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q160" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R160" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S160" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T160" t="n">
         <v>0</v>
@@ -31041,7 +31045,7 @@
         <v>0</v>
       </c>
       <c r="W160" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X160" t="inlineStr">
         <is>
@@ -31110,19 +31114,19 @@
         <v>0</v>
       </c>
       <c r="O161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P161" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q161" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="R161" t="n">
-        <v>178500</v>
+        <v>357000</v>
       </c>
       <c r="S161" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="T161" t="n">
         <v>0</v>
@@ -31134,7 +31138,7 @@
         <v>0</v>
       </c>
       <c r="W161" t="n">
-        <v>198500</v>
+        <v>397000</v>
       </c>
       <c r="X161" t="inlineStr">
         <is>
@@ -34216,16 +34220,16 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
@@ -34396,7 +34400,7 @@
         </is>
       </c>
       <c r="H11" s="18" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -34469,7 +34473,7 @@
         </is>
       </c>
       <c r="G14" s="15" t="n">
-        <v>8.5</v>
+        <v>17</v>
       </c>
       <c r="H14" s="15" t="n"/>
       <c r="I14" s="7" t="n">
@@ -34506,7 +34510,7 @@
         </is>
       </c>
       <c r="G15" s="15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="15" t="inlineStr">
         <is>

</xml_diff>